<commit_message>
feat(drag and drop), fix(post api): added drag and drop functionality for todos, fixed data persistance issue in excel sheet, using local storage for the data persistance
</commit_message>
<xml_diff>
--- a/todo.xlsx
+++ b/todo.xlsx
@@ -1,59 +1,41 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <workbookPr codeName="ThisWorkbook"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Software Works\Front End Mentor - Intermediate\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37830A17-CAA2-41EA-A114-9D0D97062839}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
-  <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
-  </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
-  <si>
-    <t>id</t>
-  </si>
-  <si>
-    <t>task</t>
-  </si>
-  <si>
-    <t>isCompleted</t>
-  </si>
-  <si>
-    <t>5f05843d-2ace-4cdb-86c9-cbab74e16526</t>
-  </si>
-  <si>
-    <t>c359a92d-282a-42a2-afaf-51e6dab0fde7</t>
-  </si>
-  <si>
-    <t>61b268e6-f264-4963-a5d9-e2acda9a1659</t>
-  </si>
-  <si>
-    <t>Jog early morning</t>
-  </si>
-  <si>
-    <t>Read book for 1 hr</t>
-  </si>
-  <si>
-    <t>Jump off the building</t>
-  </si>
-</sst>
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:vt="http://schemas.openxmlformats.org/officeDocument/2006/docPropsVTypes">
+  <numFmts count="1">
+    <numFmt numFmtId="56" formatCode="&quot;上午/下午 &quot;hh&quot;時&quot;mm&quot;分&quot;ss&quot;秒 &quot;"/>
+  </numFmts>
+  <fonts count="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -90,14 +72,6 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -422,64 +396,93 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
-    </sheetView>
+    <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" t="s">
-        <v>6</v>
+    <row r="1">
+      <c r="A1" t="str">
+        <v>id</v>
+      </c>
+      <c r="B1" t="str">
+        <v>task</v>
+      </c>
+      <c r="C1" t="str">
+        <v>isCompleted</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="str">
+        <v>5f05843d-2ace-4cdb-86c9-cbab74e16526</v>
+      </c>
+      <c r="B2" t="str">
+        <v>Jog early morning</v>
       </c>
       <c r="C2" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" t="s">
-        <v>7</v>
+    <row r="3">
+      <c r="A3" t="str">
+        <v>c359a92d-282a-42a2-afaf-51e6dab0fde7</v>
+      </c>
+      <c r="B3" t="str">
+        <v>Read book for 1 hr</v>
       </c>
       <c r="C3" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" t="s">
-        <v>8</v>
+    <row r="4">
+      <c r="A4" t="str">
+        <v>61b268e6-f264-4963-a5d9-e2acda9a1659</v>
+      </c>
+      <c r="B4" t="str">
+        <v>Jump off the building</v>
       </c>
       <c r="C4" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="15.75" x14ac:dyDescent="0.25"/>
+    <row r="5">
+      <c r="A5" t="str">
+        <v>c3a18998-4432-473b-950a-7943003c0a6e</v>
+      </c>
+      <c r="B5" t="str">
+        <v>this is a task</v>
+      </c>
+      <c r="C5" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="str">
+        <v>80fc3588-1dcf-4e4e-8d3b-4520758457f9</v>
+      </c>
+      <c r="B6" t="str">
+        <v>this is a task</v>
+      </c>
+      <c r="C6" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="str">
+        <v>5d8abbcb-a305-487a-9872-8f8f75cd31e4</v>
+      </c>
+      <c r="B7" t="str">
+        <v>this is a task</v>
+      </c>
+      <c r="C7" t="b">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="A1:C1 A4 A2 A3 C3 C4" numberStoredAsText="1"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:C7"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>